<commit_message>
Aggiunto warning per veicoli non in estrazione ed escluse relative commesse
</commit_message>
<xml_diff>
--- a/PS-VRP/Dati_output/euristico_costruttivo.xlsx
+++ b/PS-VRP/Dati_output/euristico_costruttivo.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R30"/>
+  <dimension ref="A1:R27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -813,7 +813,7 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>251453</v>
+        <v>251396</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -821,10 +821,10 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D6" t="n">
-        <v>78.125</v>
+        <v>35.34375</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -833,21 +833,21 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2025-05-07 11:58:45</t>
+          <t>2025-05-07 12:00:45</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>2025-05-07 11:58:45</t>
+          <t>2025-05-07 12:00:45</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>2025-05-07 13:16:52</t>
+          <t>2025-05-07 12:36:05</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>5000</v>
+        <v>2262</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -860,15 +860,13 @@
         </is>
       </c>
       <c r="L6" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="M6" t="n">
         <v>70</v>
       </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>39742 (non in estrazione)</t>
-        </is>
+      <c r="N6" t="n">
+        <v>39749</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
@@ -876,20 +874,20 @@
         </is>
       </c>
       <c r="P6" t="n">
-        <v>39742</v>
+        <v>39749</v>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>2025-04-28 00:00:00</t>
+          <t>2025-05-02 00:00:00</t>
         </is>
       </c>
       <c r="R6" s="1" t="n">
-        <v>-9.553385416666666</v>
+        <v>-0.5250651041666666</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>251396</v>
+        <v>251548</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -897,33 +895,33 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D7" t="n">
-        <v>35.34375</v>
+        <v>206.90625</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2025-05-07 13:16:52</t>
+          <t>2025-05-07 12:36:05</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2025-05-07 13:37:52</t>
+          <t>2025-05-07 12:55:05</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>2025-05-07 13:37:52</t>
+          <t>2025-05-07 12:55:05</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>2025-05-07 14:13:13</t>
+          <t>2025-05-08 08:22:00</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>2262</v>
+        <v>13242</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -936,7 +934,7 @@
         </is>
       </c>
       <c r="L7" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M7" t="n">
         <v>70</v>
@@ -954,50 +952,50 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>2025-05-02 00:00:00</t>
+          <t>2025-05-06 00:00:00</t>
         </is>
       </c>
       <c r="R7" s="1" t="n">
-        <v>-0.5925130208333333</v>
+        <v>-1.348611111111111</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>251548</v>
+        <v>251547</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="D8" t="n">
-        <v>206.90625</v>
+        <v>184.9154929577465</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2025-05-07 14:13:13</t>
+          <t>2025-05-08 07:00:00</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2025-05-07 14:32:13</t>
+          <t>2025-05-08 07:34:00</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>2025-05-07 14:32:13</t>
+          <t>2025-05-08 07:34:00</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>2025-05-08 09:59:07</t>
+          <t>2025-05-08 10:38:54</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>13242</v>
+        <v>13129</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1032,23 +1030,23 @@
         </is>
       </c>
       <c r="R8" s="1" t="n">
-        <v>-1.416059027777778</v>
+        <v>-1.443691314548611</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>251547</v>
+        <v>251742</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D9" t="n">
-        <v>184.9154929577465</v>
+        <v>134.8524590163935</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -1057,21 +1055,21 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2025-05-08 07:34:00</t>
+          <t>2025-05-08 07:30:00</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>2025-05-08 07:34:00</t>
+          <t>2025-05-08 07:30:00</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>2025-05-08 10:38:54</t>
+          <t>2025-05-08 09:44:51</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>13129</v>
+        <v>8226</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1102,27 +1100,27 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>2025-05-06 00:00:00</t>
+          <t>2025-05-15 00:00:00</t>
         </is>
       </c>
       <c r="R9" s="1" t="n">
-        <v>-1.443691314548611</v>
+        <v>-1.406147540983796</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>251742</v>
+        <v>251164</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="D10" t="n">
-        <v>134.8524590163935</v>
+        <v>204.0816326530612</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -1131,21 +1129,21 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2025-05-08 07:30:00</t>
+          <t>2025-05-08 07:55:00</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>2025-05-08 07:30:00</t>
+          <t>2025-05-08 07:55:00</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>2025-05-08 09:44:51</t>
+          <t>2025-05-08 11:19:04</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>8226</v>
+        <v>10000</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -1158,7 +1156,7 @@
         </is>
       </c>
       <c r="L10" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M10" t="n">
         <v>70</v>
@@ -1176,50 +1174,50 @@
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>2025-05-15 00:00:00</t>
+          <t>2025-04-22 00:00:00</t>
         </is>
       </c>
       <c r="R10" s="1" t="n">
-        <v>-1.406147540983796</v>
+        <v>-1.471584467118056</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>251268</v>
+        <v>250923</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>109.46875</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2025-05-08 07:00:00</t>
+          <t>2025-05-08 08:22:00</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2025-05-08 07:47:00</t>
+          <t>2025-05-08 08:54:00</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>2025-05-08 07:47:00</t>
+          <t>2025-05-08 08:54:00</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>2025-05-08 07:47:00</t>
+          <t>2025-05-08 10:43:28</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>0</v>
+        <v>7006</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -1228,19 +1226,17 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L11" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M11" t="n">
         <v>76</v>
       </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>39666 (non in estrazione)</t>
-        </is>
+      <c r="N11" t="n">
+        <v>39749</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
@@ -1248,54 +1244,54 @@
         </is>
       </c>
       <c r="P11" t="n">
-        <v>39666</v>
+        <v>39749</v>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>2025-04-14 00:00:00</t>
+          <t>2025-04-07 00:00:00</t>
         </is>
       </c>
       <c r="R11" s="1" t="n">
-        <v>-24.32430555555555</v>
+        <v>-1.446853298611111</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>251164</v>
+        <v>251840</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="D12" t="n">
-        <v>204.0816326530612</v>
+        <v>93.67213114754098</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2025-05-08 07:47:00</t>
+          <t>2025-05-08 09:44:51</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2025-05-08 08:34:00</t>
+          <t>2025-05-08 10:09:51</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>2025-05-08 08:34:00</t>
+          <t>2025-05-08 10:09:51</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>2025-05-08 11:58:04</t>
+          <t>2025-05-08 11:43:31</t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>10000</v>
+        <v>5714</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1308,13 +1304,13 @@
         </is>
       </c>
       <c r="L12" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M12" t="n">
         <v>70</v>
       </c>
       <c r="N12" t="n">
-        <v>39749</v>
+        <v>39758</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
@@ -1322,54 +1318,54 @@
         </is>
       </c>
       <c r="P12" t="n">
-        <v>39749</v>
+        <v>39758</v>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>2025-04-22 00:00:00</t>
+          <t>2025-05-09 00:00:00</t>
         </is>
       </c>
       <c r="R12" s="1" t="n">
-        <v>-1.498667800451389</v>
+        <v>-0.4885587431712963</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>251840</v>
+        <v>250759</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D13" t="n">
-        <v>93.67213114754098</v>
+        <v>118.2816901408451</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2025-05-08 09:44:51</t>
+          <t>2025-05-08 10:38:54</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2025-05-08 10:09:51</t>
+          <t>2025-05-08 11:08:54</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>2025-05-08 10:09:51</t>
+          <t>2025-05-08 11:08:54</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>2025-05-08 11:43:31</t>
+          <t>2025-05-08 13:07:11</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>5714</v>
+        <v>8398</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1378,17 +1374,17 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12</t>
         </is>
       </c>
       <c r="L13" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M13" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N13" t="n">
-        <v>39758</v>
+        <v>39747</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
@@ -1396,20 +1392,20 @@
         </is>
       </c>
       <c r="P13" t="n">
-        <v>39758</v>
+        <v>39747</v>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>2025-05-09 00:00:00</t>
+          <t>2025-03-13 00:00:00</t>
         </is>
       </c>
       <c r="R13" s="1" t="n">
-        <v>-0.4885587431712963</v>
+        <v>-0.5466647104861111</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>250923</v>
+        <v>251477</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -1417,33 +1413,33 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="D14" t="n">
-        <v>109.46875</v>
+        <v>468.734375</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2025-05-08 09:59:07</t>
+          <t>2025-05-08 10:43:28</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2025-05-08 10:31:07</t>
+          <t>2025-05-08 11:02:28</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>2025-05-08 10:31:07</t>
+          <t>2025-05-08 11:02:28</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>2025-05-08 12:20:35</t>
+          <t>2025-05-09 10:51:12</t>
         </is>
       </c>
       <c r="I14" t="n">
-        <v>7006</v>
+        <v>29999</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1452,17 +1448,17 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L14" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M14" t="n">
         <v>76</v>
       </c>
       <c r="N14" t="n">
-        <v>39749</v>
+        <v>39760</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
@@ -1470,54 +1466,54 @@
         </is>
       </c>
       <c r="P14" t="n">
-        <v>39749</v>
+        <v>39760</v>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>2025-04-07 00:00:00</t>
+          <t>2025-04-28 00:00:00</t>
         </is>
       </c>
       <c r="R14" s="1" t="n">
-        <v>-1.514301215277778</v>
+        <v>-2.452224392361111</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>250759</v>
+        <v>251456</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="D15" t="n">
-        <v>118.2816901408451</v>
+        <v>183.6530612244898</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2025-05-08 10:38:54</t>
+          <t>2025-05-08 11:19:04</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2025-05-08 11:08:54</t>
+          <t>2025-05-08 12:09:04</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>2025-05-08 11:08:54</t>
+          <t>2025-05-08 12:09:04</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>2025-05-08 13:07:11</t>
+          <t>2025-05-09 07:12:44</t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>8398</v>
+        <v>8999</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1526,17 +1522,17 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L15" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M15" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N15" t="n">
-        <v>39747</v>
+        <v>39746</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -1544,20 +1540,20 @@
         </is>
       </c>
       <c r="P15" t="n">
-        <v>39747</v>
+        <v>39746</v>
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>2025-03-13 00:00:00</t>
+          <t>2025-05-09 00:00:00</t>
         </is>
       </c>
       <c r="R15" s="1" t="n">
-        <v>-0.5466647104861111</v>
+        <v>-3.300510204085648</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>251456</v>
+        <v>251229</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -1565,10 +1561,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D16" t="n">
-        <v>147.5245901639344</v>
+        <v>307.1967213114754</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -1577,21 +1573,21 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2025-05-08 12:13:31</t>
+          <t>2025-05-08 12:08:31</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>2025-05-08 12:13:31</t>
+          <t>2025-05-08 12:08:31</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>2025-05-08 14:41:02</t>
+          <t>2025-05-09 09:15:43</t>
         </is>
       </c>
       <c r="I16" t="n">
-        <v>8999</v>
+        <v>18739</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -1600,17 +1596,19 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R9</t>
         </is>
       </c>
       <c r="L16" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="M16" t="n">
         <v>70</v>
       </c>
-      <c r="N16" t="n">
-        <v>39746</v>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>39723 (esterno)</t>
+        </is>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -1618,20 +1616,20 @@
         </is>
       </c>
       <c r="P16" t="n">
-        <v>39746</v>
+        <v>39723</v>
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>2025-05-09 00:00:00</t>
+          <t>2025-05-15 00:00:00</t>
         </is>
       </c>
       <c r="R16" s="1" t="n">
-        <v>-2.611839708564815</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>251477</v>
+        <v>251225</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -1639,10 +1637,10 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D17" t="n">
-        <v>422.5211267605634</v>
+        <v>0</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -1651,21 +1649,21 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2025-05-08 12:17:00</t>
+          <t>2025-05-08 12:19:00</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>2025-05-08 12:17:00</t>
+          <t>2025-05-08 12:19:00</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>2025-05-09 11:19:31</t>
+          <t>2025-05-08 12:19:00</t>
         </is>
       </c>
       <c r="I17" t="n">
-        <v>29999</v>
+        <v>0</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -1674,17 +1672,17 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L17" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M17" t="n">
         <v>76</v>
       </c>
       <c r="N17" t="n">
-        <v>39760</v>
+        <v>39747</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
@@ -1692,50 +1690,50 @@
         </is>
       </c>
       <c r="P17" t="n">
-        <v>39760</v>
+        <v>39747</v>
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>2025-04-28 00:00:00</t>
+          <t>2025-04-30 00:00:00</t>
         </is>
       </c>
       <c r="R17" s="1" t="n">
-        <v>-2.471889671365741</v>
+        <v>-0.5131944444444444</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>251225</v>
+        <v>251227</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D18" t="n">
         <v>0</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2025-05-08 12:20:35</t>
+          <t>2025-05-08 12:19:00</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2025-05-08 12:37:35</t>
+          <t>2025-05-08 12:34:00</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>2025-05-08 12:37:35</t>
+          <t>2025-05-08 12:34:00</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>2025-05-08 12:37:35</t>
+          <t>2025-05-08 12:34:00</t>
         </is>
       </c>
       <c r="I18" t="n">
@@ -1758,7 +1756,7 @@
         <v>76</v>
       </c>
       <c r="N18" t="n">
-        <v>39747</v>
+        <v>39746</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
@@ -1766,54 +1764,54 @@
         </is>
       </c>
       <c r="P18" t="n">
-        <v>39747</v>
+        <v>39746</v>
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>2025-04-30 00:00:00</t>
+          <t>2025-05-05 00:00:00</t>
         </is>
       </c>
       <c r="R18" s="1" t="n">
-        <v>-0.5261067708333333</v>
+        <v>-2.523611111111111</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>251227</v>
+        <v>251782</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D19" t="n">
-        <v>0</v>
+        <v>170.0422535211268</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2025-05-08 12:37:35</t>
+          <t>2025-05-08 12:34:00</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2025-05-08 12:52:35</t>
+          <t>2025-05-08 12:51:00</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>2025-05-08 12:52:35</t>
+          <t>2025-05-08 12:51:00</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>2025-05-08 12:52:35</t>
+          <t>2025-05-09 07:41:02</t>
         </is>
       </c>
       <c r="I19" t="n">
-        <v>0</v>
+        <v>12073</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -1822,17 +1820,17 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L19" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M19" t="n">
         <v>76</v>
       </c>
       <c r="N19" t="n">
-        <v>39746</v>
+        <v>39754</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
@@ -1840,54 +1838,54 @@
         </is>
       </c>
       <c r="P19" t="n">
-        <v>39746</v>
+        <v>39754</v>
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>2025-05-05 00:00:00</t>
+          <t>2025-05-16 00:00:00</t>
         </is>
       </c>
       <c r="R19" s="1" t="n">
-        <v>-2.5365234375</v>
+        <v>-0.3201682316087963</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>251421</v>
+        <v>251284</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>17</v>
+        <v>40.5</v>
       </c>
       <c r="D20" t="n">
-        <v>81.9375</v>
+        <v>297.0909090909091</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2025-05-08 12:52:35</t>
+          <t>2025-05-09 07:00:00</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>2025-05-08 13:09:35</t>
+          <t>2025-05-09 07:40:30</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>2025-05-08 13:09:35</t>
+          <t>2025-05-09 07:40:30</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>2025-05-08 14:31:31</t>
+          <t>2025-05-09 12:37:35</t>
         </is>
       </c>
       <c r="I20" t="n">
-        <v>5244</v>
+        <v>16340</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -1896,19 +1894,17 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
+          <t>CASON ;R6</t>
         </is>
       </c>
       <c r="L20" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="M20" t="n">
-        <v>76</v>
-      </c>
-      <c r="N20" t="inlineStr">
-        <is>
-          <t>39762 (non in estrazione)</t>
-        </is>
+        <v>70</v>
+      </c>
+      <c r="N20" t="n">
+        <v>39747</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
@@ -1916,54 +1912,54 @@
         </is>
       </c>
       <c r="P20" t="n">
-        <v>39762</v>
+        <v>39747</v>
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>2025-05-08 00:00:00</t>
+          <t>2025-05-12 00:00:00</t>
         </is>
       </c>
       <c r="R20" s="1" t="n">
-        <v>-0.6052300347222223</v>
+        <v>-1.526104797974537</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>251229</v>
+        <v>251050</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>34</v>
+        <v>217</v>
       </c>
       <c r="D21" t="n">
-        <v>263.9295774647887</v>
+        <v>0</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2025-05-08 13:07:11</t>
+          <t>2025-05-09 07:00:00</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>2025-05-08 13:41:11</t>
+          <t>2025-05-09 10:37:00</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>2025-05-08 13:41:11</t>
+          <t>2025-05-09 10:37:00</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>2025-05-09 10:05:07</t>
+          <t>2025-05-09 10:37:00</t>
         </is>
       </c>
       <c r="I21" t="n">
-        <v>18739</v>
+        <v>0</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -1972,19 +1968,17 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R9</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="L21" t="n">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="M21" t="n">
         <v>70</v>
       </c>
-      <c r="N21" t="inlineStr">
-        <is>
-          <t>39723 (esterno)</t>
-        </is>
+      <c r="N21" t="n">
+        <v>39747</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
@@ -1992,54 +1986,54 @@
         </is>
       </c>
       <c r="P21" t="n">
-        <v>39723</v>
+        <v>39747</v>
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>2025-05-15 00:00:00</t>
+          <t>2025-04-16 00:00:00</t>
         </is>
       </c>
       <c r="R21" s="1" t="n">
-        <v>0</v>
+        <v>-1.442361111111111</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>251782</v>
+        <v>251054</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="D22" t="n">
-        <v>188.640625</v>
+        <v>0</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2025-05-08 14:31:31</t>
+          <t>2025-05-09 10:37:00</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>2025-05-08 14:46:31</t>
+          <t>2025-05-09 11:12:00</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>2025-05-08 14:46:31</t>
+          <t>2025-05-09 11:12:00</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>2025-05-09 09:55:10</t>
+          <t>2025-05-09 11:12:00</t>
         </is>
       </c>
       <c r="I22" t="n">
-        <v>12073</v>
+        <v>0</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2048,17 +2042,17 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="L22" t="n">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="M22" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N22" t="n">
-        <v>39754</v>
+        <v>39747</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
@@ -2066,54 +2060,54 @@
         </is>
       </c>
       <c r="P22" t="n">
-        <v>39754</v>
+        <v>39747</v>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>2025-05-16 00:00:00</t>
+          <t>2025-04-16 00:00:00</t>
         </is>
       </c>
       <c r="R22" s="1" t="n">
-        <v>-0.4133138020833333</v>
+        <v>-1.466666666666667</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>251284</v>
+        <v>251081</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>40.5</v>
+        <v>125</v>
       </c>
       <c r="D23" t="n">
-        <v>297.0909090909091</v>
+        <v>42.42253521126761</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2025-05-09 07:00:00</t>
+          <t>2025-05-09 11:12:00</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>2025-05-09 07:40:30</t>
+          <t>2025-05-09 13:17:00</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>2025-05-09 07:40:30</t>
+          <t>2025-05-09 13:17:00</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>2025-05-09 12:37:35</t>
+          <t>2025-05-09 13:59:25</t>
         </is>
       </c>
       <c r="I23" t="n">
-        <v>16340</v>
+        <v>3012</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2122,17 +2116,19 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>CASON ;R6</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="L23" t="n">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="M23" t="n">
         <v>70</v>
       </c>
-      <c r="N23" t="n">
-        <v>39747</v>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>39750 (esterno)</t>
+        </is>
       </c>
       <c r="O23" t="inlineStr">
         <is>
@@ -2140,73 +2136,75 @@
         </is>
       </c>
       <c r="P23" t="n">
-        <v>39747</v>
+        <v>39750</v>
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>2025-05-12 00:00:00</t>
+          <t>2025-04-23 00:00:00</t>
         </is>
       </c>
       <c r="R23" s="1" t="n">
-        <v>-1.526104797974537</v>
+        <v>-16.58293231612268</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>251050</v>
+        <v>251706</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>T3</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>217</v>
+        <v>0</v>
       </c>
       <c r="D24" t="n">
+        <v>50.79365079365079</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>2025-05-12 07:00:00</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>2025-05-12 07:00:00</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>2025-05-12 07:00:00</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>2025-05-12 07:50:47</t>
+        </is>
+      </c>
+      <c r="I24" t="n">
+        <v>3200</v>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>foglio</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>T3</t>
+        </is>
+      </c>
+      <c r="L24" t="n">
         <v>0</v>
       </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>2025-05-09 07:00:00</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>2025-05-09 10:37:00</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>2025-05-09 10:37:00</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>2025-05-09 10:37:00</t>
-        </is>
-      </c>
-      <c r="I24" t="n">
+      <c r="M24" t="n">
         <v>0</v>
       </c>
-      <c r="J24" t="inlineStr">
-        <is>
-          <t>bobina</t>
-        </is>
-      </c>
-      <c r="K24" t="inlineStr">
-        <is>
-          <t>R6</t>
-        </is>
-      </c>
-      <c r="L24" t="n">
-        <v>38</v>
-      </c>
-      <c r="M24" t="n">
-        <v>70</v>
-      </c>
-      <c r="N24" t="n">
-        <v>39747</v>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>39764 (esterno)</t>
+        </is>
       </c>
       <c r="O24" t="inlineStr">
         <is>
@@ -2214,128 +2212,126 @@
         </is>
       </c>
       <c r="P24" t="n">
-        <v>39747</v>
+        <v>39764</v>
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>2025-04-16 00:00:00</t>
+          <t>2025-05-14 00:00:00</t>
         </is>
       </c>
       <c r="R24" s="1" t="n">
-        <v>-1.442361111111111</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>251054</v>
+        <v>250894</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="D25" t="n">
+        <v>623.4084507042254</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>2025-05-08 13:07:11</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>2025-05-08 13:24:11</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>2025-05-08 13:24:11</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>2025-05-12 07:47:36</t>
+        </is>
+      </c>
+      <c r="I25" t="n">
+        <v>44262</v>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>bobina</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
+        </is>
+      </c>
+      <c r="L25" t="n">
+        <v>5</v>
+      </c>
+      <c r="M25" t="n">
+        <v>76</v>
+      </c>
+      <c r="N25" t="n">
+        <v>39755</v>
+      </c>
+      <c r="O25" t="n">
         <v>0</v>
       </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>2025-05-09 10:37:00</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>2025-05-09 11:12:00</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>2025-05-09 11:12:00</t>
-        </is>
-      </c>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t>2025-05-09 11:12:00</t>
-        </is>
-      </c>
-      <c r="I25" t="n">
+      <c r="P25" t="n">
         <v>0</v>
       </c>
-      <c r="J25" t="inlineStr">
-        <is>
-          <t>bobina</t>
-        </is>
-      </c>
-      <c r="K25" t="inlineStr">
-        <is>
-          <t>R6</t>
-        </is>
-      </c>
-      <c r="L25" t="n">
-        <v>38</v>
-      </c>
-      <c r="M25" t="n">
-        <v>70</v>
-      </c>
-      <c r="N25" t="n">
-        <v>39747</v>
-      </c>
-      <c r="O25" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="P25" t="n">
-        <v>39747</v>
-      </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>2025-04-16 00:00:00</t>
+          <t>2025-05-05 00:00:00</t>
         </is>
       </c>
       <c r="R25" s="1" t="n">
-        <v>-1.466666666666667</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>251081</v>
+        <v>251651</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 4</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>125</v>
+        <v>29</v>
       </c>
       <c r="D26" t="n">
-        <v>42.42253521126761</v>
+        <v>767.7049180327868</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2025-05-09 11:12:00</t>
+          <t>2025-05-09 07:00:00</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>2025-05-09 13:17:00</t>
+          <t>2025-05-09 07:29:00</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>2025-05-09 13:17:00</t>
+          <t>2025-05-09 07:29:00</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>2025-05-09 13:59:25</t>
+          <t>2025-05-12 12:16:42</t>
         </is>
       </c>
       <c r="I26" t="n">
-        <v>3012</v>
+        <v>46830</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -2344,326 +2340,102 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L26" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="M26" t="n">
-        <v>70</v>
-      </c>
-      <c r="N26" t="inlineStr">
-        <is>
-          <t>39750 (esterno)</t>
-        </is>
-      </c>
-      <c r="O26" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
+        <v>76</v>
+      </c>
+      <c r="N26" t="n">
+        <v>39755</v>
+      </c>
+      <c r="O26" t="n">
+        <v>0</v>
       </c>
       <c r="P26" t="n">
-        <v>39750</v>
+        <v>0</v>
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>2025-04-23 00:00:00</t>
+          <t>2025-05-12 00:00:00</t>
         </is>
       </c>
       <c r="R26" s="1" t="n">
-        <v>-16.58293231612268</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>251706</v>
+        <v>251416</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>T3</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C27" t="n">
+        <v>40</v>
+      </c>
+      <c r="D27" t="n">
+        <v>229.0204081632653</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>2025-05-09 07:12:44</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>2025-05-09 07:52:44</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>2025-05-09 07:52:44</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>2025-05-09 11:41:45</t>
+        </is>
+      </c>
+      <c r="I27" t="n">
+        <v>11222</v>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>bobina</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+        </is>
+      </c>
+      <c r="L27" t="n">
+        <v>2</v>
+      </c>
+      <c r="M27" t="n">
+        <v>70</v>
+      </c>
+      <c r="N27" t="n">
+        <v>39755</v>
+      </c>
+      <c r="O27" t="n">
         <v>0</v>
       </c>
-      <c r="D27" t="n">
-        <v>50.79365079365079</v>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>2025-05-12 07:00:00</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>2025-05-12 07:00:00</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>2025-05-12 07:00:00</t>
-        </is>
-      </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>2025-05-12 07:50:47</t>
-        </is>
-      </c>
-      <c r="I27" t="n">
-        <v>3200</v>
-      </c>
-      <c r="J27" t="inlineStr">
-        <is>
-          <t>foglio</t>
-        </is>
-      </c>
-      <c r="K27" t="inlineStr">
-        <is>
-          <t>T3</t>
-        </is>
-      </c>
-      <c r="L27" t="n">
+      <c r="P27" t="n">
         <v>0</v>
       </c>
-      <c r="M27" t="n">
-        <v>0</v>
-      </c>
-      <c r="N27" t="inlineStr">
-        <is>
-          <t>39764 (esterno)</t>
-        </is>
-      </c>
-      <c r="O27" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="P27" t="n">
-        <v>39764</v>
-      </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>2025-05-14 00:00:00</t>
+          <t>2025-04-23 00:00:00</t>
         </is>
       </c>
       <c r="R27" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="n">
-        <v>250894</v>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>R3</t>
-        </is>
-      </c>
-      <c r="C28" t="n">
-        <v>42</v>
-      </c>
-      <c r="D28" t="n">
-        <v>903.3061224489796</v>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>2025-05-08 11:58:04</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>2025-05-08 12:40:04</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>2025-05-08 12:40:04</t>
-        </is>
-      </c>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t>2025-05-12 11:43:23</t>
-        </is>
-      </c>
-      <c r="I28" t="n">
-        <v>44262</v>
-      </c>
-      <c r="J28" t="inlineStr">
-        <is>
-          <t>bobina</t>
-        </is>
-      </c>
-      <c r="K28" t="inlineStr">
-        <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
-        </is>
-      </c>
-      <c r="L28" t="n">
-        <v>5</v>
-      </c>
-      <c r="M28" t="n">
-        <v>76</v>
-      </c>
-      <c r="N28" t="n">
-        <v>39755</v>
-      </c>
-      <c r="O28" t="n">
-        <v>0</v>
-      </c>
-      <c r="P28" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q28" t="inlineStr">
-        <is>
-          <t>2025-05-05 00:00:00</t>
-        </is>
-      </c>
-      <c r="R28" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="n">
-        <v>251416</v>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>R10</t>
-        </is>
-      </c>
-      <c r="C29" t="n">
-        <v>25</v>
-      </c>
-      <c r="D29" t="n">
-        <v>183.9672131147541</v>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>2025-05-08 14:41:02</t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>2025-05-09 07:06:02</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>2025-05-09 07:06:02</t>
-        </is>
-      </c>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t>2025-05-09 10:10:00</t>
-        </is>
-      </c>
-      <c r="I29" t="n">
-        <v>11222</v>
-      </c>
-      <c r="J29" t="inlineStr">
-        <is>
-          <t>bobina</t>
-        </is>
-      </c>
-      <c r="K29" t="inlineStr">
-        <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
-        </is>
-      </c>
-      <c r="L29" t="n">
-        <v>2</v>
-      </c>
-      <c r="M29" t="n">
-        <v>70</v>
-      </c>
-      <c r="N29" t="n">
-        <v>39755</v>
-      </c>
-      <c r="O29" t="n">
-        <v>0</v>
-      </c>
-      <c r="P29" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q29" t="inlineStr">
-        <is>
-          <t>2025-04-23 00:00:00</t>
-        </is>
-      </c>
-      <c r="R29" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="n">
-        <v>251651</v>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>BIMEC 4</t>
-        </is>
-      </c>
-      <c r="C30" t="n">
-        <v>29</v>
-      </c>
-      <c r="D30" t="n">
-        <v>767.7049180327868</v>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>2025-05-09 07:00:00</t>
-        </is>
-      </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>2025-05-09 07:29:00</t>
-        </is>
-      </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>2025-05-09 07:29:00</t>
-        </is>
-      </c>
-      <c r="H30" t="inlineStr">
-        <is>
-          <t>2025-05-12 12:16:42</t>
-        </is>
-      </c>
-      <c r="I30" t="n">
-        <v>46830</v>
-      </c>
-      <c r="J30" t="inlineStr">
-        <is>
-          <t>bobina</t>
-        </is>
-      </c>
-      <c r="K30" t="inlineStr">
-        <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
-        </is>
-      </c>
-      <c r="L30" t="n">
-        <v>5</v>
-      </c>
-      <c r="M30" t="n">
-        <v>76</v>
-      </c>
-      <c r="N30" t="n">
-        <v>39755</v>
-      </c>
-      <c r="O30" t="n">
-        <v>0</v>
-      </c>
-      <c r="P30" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q30" t="inlineStr">
-        <is>
-          <t>2025-05-12 00:00:00</t>
-        </is>
-      </c>
-      <c r="R30" s="1" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Prima prova di introduzione della funzione obiettivo in una ricerca locale (insert intramacchina - LS2)
</commit_message>
<xml_diff>
--- a/PS-VRP/Dati_output/euristico_costruttivo.xlsx
+++ b/PS-VRP/Dati_output/euristico_costruttivo.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R27"/>
+  <dimension ref="A1:S27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -586,6 +586,9 @@
       <c r="R2" s="1" t="n">
         <v>-0.3623372395833334</v>
       </c>
+      <c r="S2" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -660,6 +663,9 @@
       <c r="R3" s="1" t="n">
         <v>-0.4377821180555556</v>
       </c>
+      <c r="S3" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -734,6 +740,9 @@
       <c r="R4" s="1" t="n">
         <v>-0.4741319444444445</v>
       </c>
+      <c r="S4" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -810,6 +819,9 @@
       <c r="R5" s="1" t="n">
         <v>-13.48732638888889</v>
       </c>
+      <c r="S5" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -884,6 +896,9 @@
       <c r="R6" s="1" t="n">
         <v>-0.5250651041666666</v>
       </c>
+      <c r="S6" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -958,6 +973,9 @@
       <c r="R7" s="1" t="n">
         <v>-1.348611111111111</v>
       </c>
+      <c r="S7" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -1032,6 +1050,9 @@
       <c r="R8" s="1" t="n">
         <v>-1.443691314548611</v>
       </c>
+      <c r="S8" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1106,6 +1127,9 @@
       <c r="R9" s="1" t="n">
         <v>-1.406147540983796</v>
       </c>
+      <c r="S9" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1180,6 +1204,9 @@
       <c r="R10" s="1" t="n">
         <v>-1.471584467118056</v>
       </c>
+      <c r="S10" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1254,6 +1281,9 @@
       <c r="R11" s="1" t="n">
         <v>-1.446853298611111</v>
       </c>
+      <c r="S11" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1328,6 +1358,9 @@
       <c r="R12" s="1" t="n">
         <v>-0.4885587431712963</v>
       </c>
+      <c r="S12" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1402,6 +1435,9 @@
       <c r="R13" s="1" t="n">
         <v>-0.5466647104861111</v>
       </c>
+      <c r="S13" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1476,6 +1512,9 @@
       <c r="R14" s="1" t="n">
         <v>-2.452224392361111</v>
       </c>
+      <c r="S14" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1550,6 +1589,9 @@
       <c r="R15" s="1" t="n">
         <v>-3.300510204085648</v>
       </c>
+      <c r="S15" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1626,6 +1668,9 @@
       <c r="R16" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="S16" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1700,6 +1745,9 @@
       <c r="R17" s="1" t="n">
         <v>-0.5131944444444444</v>
       </c>
+      <c r="S17" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1774,6 +1822,9 @@
       <c r="R18" s="1" t="n">
         <v>-2.523611111111111</v>
       </c>
+      <c r="S18" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -1848,6 +1899,9 @@
       <c r="R19" s="1" t="n">
         <v>-0.3201682316087963</v>
       </c>
+      <c r="S19" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -1922,6 +1976,9 @@
       <c r="R20" s="1" t="n">
         <v>-1.526104797974537</v>
       </c>
+      <c r="S20" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -1996,6 +2053,9 @@
       <c r="R21" s="1" t="n">
         <v>-1.442361111111111</v>
       </c>
+      <c r="S21" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -2070,6 +2130,9 @@
       <c r="R22" s="1" t="n">
         <v>-1.466666666666667</v>
       </c>
+      <c r="S22" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -2146,6 +2209,9 @@
       <c r="R23" s="1" t="n">
         <v>-16.58293231612268</v>
       </c>
+      <c r="S23" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -2222,6 +2288,9 @@
       <c r="R24" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="S24" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -2294,6 +2363,9 @@
       <c r="R25" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="S25" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -2366,6 +2438,9 @@
       <c r="R26" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="S26" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -2437,6 +2512,9 @@
       </c>
       <c r="R27" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="S27" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>